<commit_message>
OG Code Refactor code to import required libraries and remove unused imports. Update script to store differences in a sheet and repeat the process. Update script to include a summary of differences in the console output. Update script to delete rows with no differences. Update script to allow user input for output file name and sheet name.
</commit_message>
<xml_diff>
--- a/PGE_Report_Field_Maps before - Copy.xlsx
+++ b/PGE_Report_Field_Maps before - Copy.xlsx
@@ -70,7 +70,7 @@
     <t>Delete Protection</t>
   </si>
   <si>
-    <t>ARM 2023 Space TEST</t>
+    <t>ARM 2023 Space</t>
   </si>
   <si>
     <t>c7654927cf554c9490fe639178351fb9</t>
@@ -97,34 +97,34 @@
     <t>Not Configured</t>
   </si>
   <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>ARM_b Transmission Roads</t>
+  </si>
+  <si>
+    <t>6003d30a5f06445897ac7facd7287480</t>
+  </si>
+  <si>
+    <t>https://pgegisportal.maps.arcgis.com/home/item.html?id=6003d30a5f06445897ac7facd7287480</t>
+  </si>
+  <si>
+    <t>All Electric Transmission Operations Map</t>
+  </si>
+  <si>
+    <t>ARM Electric Transmission @ pgegisportal, ARM LPM @ pgegisportal, Favorites - LandOperations Owner PG&amp;E_GISCOE, ARM Dev Data Team Shared Update, ESAP Telecom 2024 @ pgegisportal</t>
+  </si>
+  <si>
+    <t>BLM Administrative Boundary</t>
+  </si>
+  <si>
+    <t>eddd7c44a9814fbda72746b9309368a5</t>
+  </si>
+  <si>
+    <t>BLM Administrative Boundary: {AGENCY_SUBTITLE}</t>
+  </si>
+  <si>
     <t>Enabled</t>
-  </si>
-  <si>
-    <t>Off</t>
-  </si>
-  <si>
-    <t>ARM_b Transmission Roads</t>
-  </si>
-  <si>
-    <t>6003d30a5f06445897ac7facd7287480</t>
-  </si>
-  <si>
-    <t>https://pgegisportal.maps.arcgis.com/home/item.html?id=6003d30a5f06445897ac7facd7287480</t>
-  </si>
-  <si>
-    <t>All Electric Transmission Operations Map</t>
-  </si>
-  <si>
-    <t>ARM Electric Transmission @ pgegisportal, ARM LPM @ pgegisportal, Favorites - LandOperations Owner PG&amp;E_GISCOE, ARM Dev Data Team Shared Update, ESAP Telecom 2024 @ pgegisportal</t>
-  </si>
-  <si>
-    <t>BLM Administrative Boundary</t>
-  </si>
-  <si>
-    <t>eddd7c44a9814fbda72746b9309368a5</t>
-  </si>
-  <si>
-    <t>BLM Administrative Boundary: {AGENCY_SUBTITLE}</t>
   </si>
   <si>
     <t>On</t>
@@ -586,7 +586,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -596,6 +596,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -787,34 +793,34 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -987,9 +993,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1069,7 +1075,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1096,10 +1102,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1346,9 +1352,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1626,7 +1632,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1653,10 +1659,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2025,44 +2031,42 @@
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
-      <c r="R2" t="s" s="7">
+      <c r="R2" s="7"/>
+      <c r="S2" t="s" s="10">
         <v>28</v>
-      </c>
-      <c r="S2" t="s" s="10">
-        <v>29</v>
       </c>
       <c r="T2" s="5"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F3" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s" s="7">
         <v>34</v>
-      </c>
-      <c r="G3" t="s" s="7">
-        <v>35</v>
       </c>
       <c r="H3" t="b" s="9">
         <v>0</v>
       </c>
       <c r="I3" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s" s="7">
         <v>36</v>
-      </c>
-      <c r="J3" t="s" s="7">
-        <v>37</v>
       </c>
       <c r="K3" t="s" s="7">
         <v>27</v>
@@ -2074,7 +2078,7 @@
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S3" t="s" s="10">
         <v>38</v>
@@ -2083,22 +2087,22 @@
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F4" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s" s="7">
         <v>39</v>
@@ -2122,7 +2126,7 @@
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S4" t="s" s="10">
         <v>38</v>
@@ -2131,22 +2135,22 @@
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F5" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s" s="7">
         <v>42</v>
@@ -2170,7 +2174,7 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S5" t="s" s="10">
         <v>38</v>
@@ -2179,22 +2183,22 @@
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F6" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s" s="7">
         <v>45</v>
@@ -2218,7 +2222,7 @@
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
       <c r="R6" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S6" t="s" s="10">
         <v>38</v>
@@ -2227,22 +2231,22 @@
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F7" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s" s="7">
         <v>48</v>
@@ -2264,7 +2268,7 @@
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
       <c r="R7" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S7" t="s" s="10">
         <v>38</v>
@@ -2273,22 +2277,22 @@
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F8" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s" s="7">
         <v>50</v>
@@ -2312,7 +2316,7 @@
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
       <c r="R8" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S8" t="s" s="10">
         <v>38</v>
@@ -2321,22 +2325,22 @@
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F9" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" t="s" s="7">
         <v>52</v>
@@ -2360,7 +2364,7 @@
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
       <c r="R9" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S9" t="s" s="10">
         <v>38</v>
@@ -2369,22 +2373,22 @@
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F10" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s" s="7">
         <v>54</v>
@@ -2408,7 +2412,7 @@
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
       <c r="R10" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S10" t="s" s="10">
         <v>38</v>
@@ -2417,22 +2421,22 @@
     </row>
     <row r="11" ht="13.55" customHeight="1">
       <c r="A11" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F11" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G11" t="s" s="7">
         <v>57</v>
@@ -2456,7 +2460,7 @@
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S11" t="s" s="10">
         <v>38</v>
@@ -2465,22 +2469,22 @@
     </row>
     <row r="12" ht="13.55" customHeight="1">
       <c r="A12" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F12" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s" s="7">
         <v>60</v>
@@ -2504,7 +2508,7 @@
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
       <c r="R12" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S12" t="s" s="10">
         <v>38</v>
@@ -2513,22 +2517,22 @@
     </row>
     <row r="13" ht="13.55" customHeight="1">
       <c r="A13" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F13" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G13" t="s" s="7">
         <v>63</v>
@@ -2560,7 +2564,7 @@
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S13" t="s" s="10">
         <v>38</v>
@@ -2569,22 +2573,22 @@
     </row>
     <row r="14" ht="13.55" customHeight="1">
       <c r="A14" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F14" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G14" t="s" s="7">
         <v>63</v>
@@ -2618,7 +2622,7 @@
         <v>75</v>
       </c>
       <c r="R14" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S14" t="s" s="10">
         <v>38</v>
@@ -2627,22 +2631,22 @@
     </row>
     <row r="15" ht="13.55" customHeight="1">
       <c r="A15" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F15" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G15" t="s" s="7">
         <v>63</v>
@@ -2678,7 +2682,7 @@
         <v>75</v>
       </c>
       <c r="R15" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S15" t="s" s="10">
         <v>38</v>
@@ -2687,22 +2691,22 @@
     </row>
     <row r="16" ht="13.55" customHeight="1">
       <c r="A16" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F16" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G16" t="s" s="7">
         <v>63</v>
@@ -2738,7 +2742,7 @@
         <v>75</v>
       </c>
       <c r="R16" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S16" t="s" s="10">
         <v>38</v>
@@ -2747,22 +2751,22 @@
     </row>
     <row r="17" ht="13.55" customHeight="1">
       <c r="A17" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F17" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G17" t="s" s="7">
         <v>63</v>
@@ -2794,7 +2798,7 @@
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S17" t="s" s="10">
         <v>38</v>
@@ -2803,22 +2807,22 @@
     </row>
     <row r="18" ht="13.55" customHeight="1">
       <c r="A18" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F18" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G18" t="s" s="7">
         <v>63</v>
@@ -2852,7 +2856,7 @@
         <v>75</v>
       </c>
       <c r="R18" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S18" t="s" s="10">
         <v>38</v>
@@ -2861,22 +2865,22 @@
     </row>
     <row r="19" ht="13.55" customHeight="1">
       <c r="A19" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F19" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G19" t="s" s="7">
         <v>63</v>
@@ -2910,7 +2914,7 @@
         <v>75</v>
       </c>
       <c r="R19" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S19" t="s" s="10">
         <v>38</v>
@@ -2919,22 +2923,22 @@
     </row>
     <row r="20" ht="13.55" customHeight="1">
       <c r="A20" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F20" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s" s="7">
         <v>63</v>
@@ -2968,7 +2972,7 @@
         <v>75</v>
       </c>
       <c r="R20" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S20" t="s" s="10">
         <v>38</v>
@@ -2977,22 +2981,22 @@
     </row>
     <row r="21" ht="13.55" customHeight="1">
       <c r="A21" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F21" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G21" t="s" s="7">
         <v>63</v>
@@ -3026,7 +3030,7 @@
         <v>75</v>
       </c>
       <c r="R21" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S21" t="s" s="10">
         <v>38</v>
@@ -3035,22 +3039,22 @@
     </row>
     <row r="22" ht="13.55" customHeight="1">
       <c r="A22" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F22" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G22" t="s" s="7">
         <v>63</v>
@@ -3082,7 +3086,7 @@
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
       <c r="R22" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S22" t="s" s="10">
         <v>38</v>
@@ -3091,22 +3095,22 @@
     </row>
     <row r="23" ht="13.55" customHeight="1">
       <c r="A23" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F23" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G23" t="s" s="7">
         <v>63</v>
@@ -3138,7 +3142,7 @@
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="R23" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S23" t="s" s="10">
         <v>38</v>
@@ -3147,22 +3151,22 @@
     </row>
     <row r="24" ht="13.55" customHeight="1">
       <c r="A24" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F24" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G24" t="s" s="7">
         <v>63</v>
@@ -3194,7 +3198,7 @@
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
       <c r="R24" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S24" t="s" s="10">
         <v>38</v>
@@ -3203,22 +3207,22 @@
     </row>
     <row r="25" ht="13.55" customHeight="1">
       <c r="A25" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F25" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G25" t="s" s="7">
         <v>63</v>
@@ -3250,7 +3254,7 @@
       <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
       <c r="R25" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S25" t="s" s="10">
         <v>38</v>
@@ -3259,22 +3263,22 @@
     </row>
     <row r="26" ht="13.55" customHeight="1">
       <c r="A26" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E26" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F26" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G26" t="s" s="7">
         <v>63</v>
@@ -3306,7 +3310,7 @@
       <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
       <c r="R26" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S26" t="s" s="10">
         <v>38</v>
@@ -3315,22 +3319,22 @@
     </row>
     <row r="27" ht="13.55" customHeight="1">
       <c r="A27" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E27" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F27" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G27" t="s" s="7">
         <v>63</v>
@@ -3362,7 +3366,7 @@
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
       <c r="R27" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S27" t="s" s="10">
         <v>38</v>
@@ -3371,22 +3375,22 @@
     </row>
     <row r="28" ht="13.55" customHeight="1">
       <c r="A28" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E28" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F28" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G28" t="s" s="7">
         <v>63</v>
@@ -3418,7 +3422,7 @@
       <c r="P28" s="8"/>
       <c r="Q28" s="8"/>
       <c r="R28" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S28" t="s" s="10">
         <v>38</v>
@@ -3427,22 +3431,22 @@
     </row>
     <row r="29" ht="13.55" customHeight="1">
       <c r="A29" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E29" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F29" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G29" t="s" s="7">
         <v>63</v>
@@ -3474,7 +3478,7 @@
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
       <c r="R29" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S29" t="s" s="10">
         <v>38</v>
@@ -3483,22 +3487,22 @@
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E30" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F30" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G30" t="s" s="7">
         <v>63</v>
@@ -3530,7 +3534,7 @@
       <c r="P30" s="8"/>
       <c r="Q30" s="8"/>
       <c r="R30" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S30" t="s" s="10">
         <v>38</v>
@@ -3539,22 +3543,22 @@
     </row>
     <row r="31" ht="13.55" customHeight="1">
       <c r="A31" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E31" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F31" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G31" t="s" s="7">
         <v>63</v>
@@ -3586,7 +3590,7 @@
       <c r="P31" s="8"/>
       <c r="Q31" s="8"/>
       <c r="R31" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S31" t="s" s="10">
         <v>38</v>
@@ -3595,22 +3599,22 @@
     </row>
     <row r="32" ht="13.55" customHeight="1">
       <c r="A32" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E32" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F32" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G32" t="s" s="7">
         <v>63</v>
@@ -3642,7 +3646,7 @@
       <c r="P32" s="8"/>
       <c r="Q32" s="8"/>
       <c r="R32" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S32" t="s" s="10">
         <v>38</v>
@@ -3651,22 +3655,22 @@
     </row>
     <row r="33" ht="13.55" customHeight="1">
       <c r="A33" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E33" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F33" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G33" t="s" s="7">
         <v>115</v>
@@ -3698,7 +3702,7 @@
       <c r="P33" s="8"/>
       <c r="Q33" s="8"/>
       <c r="R33" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S33" t="s" s="10">
         <v>38</v>
@@ -3707,22 +3711,22 @@
     </row>
     <row r="34" ht="13.55" customHeight="1">
       <c r="A34" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E34" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F34" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G34" t="s" s="7">
         <v>115</v>
@@ -3756,7 +3760,7 @@
         <v>75</v>
       </c>
       <c r="R34" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S34" t="s" s="10">
         <v>38</v>
@@ -3765,22 +3769,22 @@
     </row>
     <row r="35" ht="13.55" customHeight="1">
       <c r="A35" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E35" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F35" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G35" t="s" s="7">
         <v>115</v>
@@ -3816,7 +3820,7 @@
         <v>75</v>
       </c>
       <c r="R35" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S35" t="s" s="10">
         <v>38</v>
@@ -3825,22 +3829,22 @@
     </row>
     <row r="36" ht="13.55" customHeight="1">
       <c r="A36" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C36" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E36" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F36" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G36" t="s" s="7">
         <v>115</v>
@@ -3876,7 +3880,7 @@
         <v>75</v>
       </c>
       <c r="R36" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S36" t="s" s="10">
         <v>38</v>
@@ -3885,22 +3889,22 @@
     </row>
     <row r="37" ht="13.55" customHeight="1">
       <c r="A37" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D37" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E37" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F37" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G37" t="s" s="7">
         <v>115</v>
@@ -3934,7 +3938,7 @@
         <v>75</v>
       </c>
       <c r="R37" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S37" t="s" s="10">
         <v>38</v>
@@ -3943,22 +3947,22 @@
     </row>
     <row r="38" ht="13.55" customHeight="1">
       <c r="A38" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D38" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E38" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F38" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G38" t="s" s="7">
         <v>115</v>
@@ -3992,7 +3996,7 @@
         <v>75</v>
       </c>
       <c r="R38" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S38" t="s" s="10">
         <v>38</v>
@@ -4001,22 +4005,22 @@
     </row>
     <row r="39" ht="13.55" customHeight="1">
       <c r="A39" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D39" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E39" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F39" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G39" t="s" s="7">
         <v>115</v>
@@ -4050,7 +4054,7 @@
         <v>75</v>
       </c>
       <c r="R39" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S39" t="s" s="10">
         <v>38</v>
@@ -4059,22 +4063,22 @@
     </row>
     <row r="40" ht="13.55" customHeight="1">
       <c r="A40" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C40" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D40" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E40" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F40" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G40" t="s" s="7">
         <v>115</v>
@@ -4106,7 +4110,7 @@
       <c r="P40" s="8"/>
       <c r="Q40" s="8"/>
       <c r="R40" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S40" t="s" s="10">
         <v>38</v>
@@ -4115,22 +4119,22 @@
     </row>
     <row r="41" ht="13.55" customHeight="1">
       <c r="A41" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C41" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D41" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E41" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F41" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G41" t="s" s="7">
         <v>115</v>
@@ -4162,7 +4166,7 @@
       <c r="P41" s="8"/>
       <c r="Q41" s="8"/>
       <c r="R41" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S41" t="s" s="10">
         <v>38</v>
@@ -4171,22 +4175,22 @@
     </row>
     <row r="42" ht="13.55" customHeight="1">
       <c r="A42" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C42" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D42" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E42" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F42" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G42" t="s" s="7">
         <v>115</v>
@@ -4218,7 +4222,7 @@
       <c r="P42" s="8"/>
       <c r="Q42" s="8"/>
       <c r="R42" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S42" t="s" s="10">
         <v>38</v>
@@ -4227,22 +4231,22 @@
     </row>
     <row r="43" ht="13.55" customHeight="1">
       <c r="A43" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C43" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D43" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E43" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F43" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G43" t="s" s="7">
         <v>115</v>
@@ -4274,7 +4278,7 @@
       <c r="P43" s="8"/>
       <c r="Q43" s="8"/>
       <c r="R43" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S43" t="s" s="10">
         <v>38</v>
@@ -4283,22 +4287,22 @@
     </row>
     <row r="44" ht="13.55" customHeight="1">
       <c r="A44" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C44" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D44" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E44" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F44" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G44" t="s" s="7">
         <v>115</v>
@@ -4330,7 +4334,7 @@
       <c r="P44" s="8"/>
       <c r="Q44" s="8"/>
       <c r="R44" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S44" t="s" s="10">
         <v>38</v>
@@ -4339,22 +4343,22 @@
     </row>
     <row r="45" ht="13.55" customHeight="1">
       <c r="A45" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D45" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E45" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F45" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G45" t="s" s="7">
         <v>115</v>
@@ -4386,7 +4390,7 @@
       <c r="P45" s="8"/>
       <c r="Q45" s="8"/>
       <c r="R45" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S45" t="s" s="10">
         <v>38</v>
@@ -4395,22 +4399,22 @@
     </row>
     <row r="46" ht="13.55" customHeight="1">
       <c r="A46" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C46" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D46" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E46" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F46" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G46" t="s" s="7">
         <v>115</v>
@@ -4444,7 +4448,7 @@
         <v>75</v>
       </c>
       <c r="R46" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S46" t="s" s="10">
         <v>38</v>
@@ -4453,22 +4457,22 @@
     </row>
     <row r="47" ht="13.55" customHeight="1">
       <c r="A47" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B47" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C47" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D47" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E47" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F47" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G47" t="s" s="7">
         <v>115</v>
@@ -4500,7 +4504,7 @@
       <c r="P47" s="8"/>
       <c r="Q47" s="8"/>
       <c r="R47" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S47" t="s" s="10">
         <v>38</v>
@@ -4509,22 +4513,22 @@
     </row>
     <row r="48" ht="13.55" customHeight="1">
       <c r="A48" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C48" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D48" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E48" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F48" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G48" t="s" s="7">
         <v>115</v>
@@ -4556,7 +4560,7 @@
       <c r="P48" s="8"/>
       <c r="Q48" s="8"/>
       <c r="R48" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S48" t="s" s="10">
         <v>38</v>
@@ -4565,22 +4569,22 @@
     </row>
     <row r="49" ht="13.55" customHeight="1">
       <c r="A49" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B49" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C49" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E49" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F49" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G49" t="s" s="7">
         <v>115</v>
@@ -4612,7 +4616,7 @@
       <c r="P49" s="8"/>
       <c r="Q49" s="8"/>
       <c r="R49" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S49" t="s" s="10">
         <v>38</v>
@@ -4621,22 +4625,22 @@
     </row>
     <row r="50" ht="13.55" customHeight="1">
       <c r="A50" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C50" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D50" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E50" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F50" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G50" t="s" s="7">
         <v>115</v>
@@ -4668,7 +4672,7 @@
       <c r="P50" s="8"/>
       <c r="Q50" s="8"/>
       <c r="R50" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S50" t="s" s="10">
         <v>38</v>
@@ -4677,22 +4681,22 @@
     </row>
     <row r="51" ht="13.55" customHeight="1">
       <c r="A51" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B51" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C51" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D51" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E51" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F51" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G51" t="s" s="7">
         <v>115</v>
@@ -4724,7 +4728,7 @@
       <c r="P51" s="8"/>
       <c r="Q51" s="8"/>
       <c r="R51" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S51" t="s" s="10">
         <v>38</v>
@@ -4733,22 +4737,22 @@
     </row>
     <row r="52" ht="13.55" customHeight="1">
       <c r="A52" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B52" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D52" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E52" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F52" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G52" t="s" s="7">
         <v>115</v>
@@ -4780,7 +4784,7 @@
       <c r="P52" s="8"/>
       <c r="Q52" s="8"/>
       <c r="R52" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S52" t="s" s="10">
         <v>38</v>
@@ -4789,22 +4793,22 @@
     </row>
     <row r="53" ht="13.55" customHeight="1">
       <c r="A53" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B53" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C53" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D53" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E53" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F53" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G53" t="s" s="7">
         <v>115</v>
@@ -4836,7 +4840,7 @@
       <c r="P53" s="8"/>
       <c r="Q53" s="8"/>
       <c r="R53" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S53" t="s" s="10">
         <v>38</v>
@@ -4845,22 +4849,22 @@
     </row>
     <row r="54" ht="13.55" customHeight="1">
       <c r="A54" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B54" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C54" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D54" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E54" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F54" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G54" t="s" s="7">
         <v>115</v>
@@ -4892,7 +4896,7 @@
       <c r="P54" s="8"/>
       <c r="Q54" s="8"/>
       <c r="R54" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S54" t="s" s="10">
         <v>38</v>
@@ -4901,22 +4905,22 @@
     </row>
     <row r="55" ht="13.55" customHeight="1">
       <c r="A55" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B55" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C55" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D55" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E55" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F55" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G55" t="s" s="7">
         <v>115</v>
@@ -4948,7 +4952,7 @@
       <c r="P55" s="8"/>
       <c r="Q55" s="8"/>
       <c r="R55" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S55" t="s" s="10">
         <v>38</v>
@@ -4957,22 +4961,22 @@
     </row>
     <row r="56" ht="13.55" customHeight="1">
       <c r="A56" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B56" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C56" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D56" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E56" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F56" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G56" t="s" s="7">
         <v>115</v>
@@ -5004,7 +5008,7 @@
       <c r="P56" s="8"/>
       <c r="Q56" s="8"/>
       <c r="R56" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S56" t="s" s="10">
         <v>38</v>
@@ -5013,22 +5017,22 @@
     </row>
     <row r="57" ht="13.55" customHeight="1">
       <c r="A57" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B57" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C57" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D57" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E57" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F57" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G57" t="s" s="7">
         <v>115</v>
@@ -5060,7 +5064,7 @@
       <c r="P57" s="8"/>
       <c r="Q57" s="8"/>
       <c r="R57" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S57" t="s" s="10">
         <v>38</v>
@@ -5069,22 +5073,22 @@
     </row>
     <row r="58" ht="13.55" customHeight="1">
       <c r="A58" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B58" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C58" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D58" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E58" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F58" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G58" t="s" s="7">
         <v>142</v>
@@ -5116,7 +5120,7 @@
       <c r="P58" s="8"/>
       <c r="Q58" s="8"/>
       <c r="R58" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S58" t="s" s="10">
         <v>38</v>
@@ -5125,22 +5129,22 @@
     </row>
     <row r="59" ht="13.55" customHeight="1">
       <c r="A59" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B59" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C59" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D59" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E59" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F59" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G59" t="s" s="7">
         <v>142</v>
@@ -5174,7 +5178,7 @@
         <v>75</v>
       </c>
       <c r="R59" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S59" t="s" s="10">
         <v>38</v>
@@ -5183,22 +5187,22 @@
     </row>
     <row r="60" ht="13.55" customHeight="1">
       <c r="A60" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B60" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C60" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D60" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E60" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F60" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G60" t="s" s="7">
         <v>142</v>
@@ -5234,7 +5238,7 @@
         <v>75</v>
       </c>
       <c r="R60" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S60" t="s" s="10">
         <v>38</v>
@@ -5243,22 +5247,22 @@
     </row>
     <row r="61" ht="13.55" customHeight="1">
       <c r="A61" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B61" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C61" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D61" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E61" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F61" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G61" t="s" s="7">
         <v>142</v>
@@ -5294,7 +5298,7 @@
         <v>75</v>
       </c>
       <c r="R61" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S61" t="s" s="10">
         <v>38</v>
@@ -5303,22 +5307,22 @@
     </row>
     <row r="62" ht="13.55" customHeight="1">
       <c r="A62" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B62" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C62" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D62" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E62" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F62" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G62" t="s" s="7">
         <v>142</v>
@@ -5352,7 +5356,7 @@
         <v>75</v>
       </c>
       <c r="R62" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S62" t="s" s="10">
         <v>38</v>
@@ -5361,22 +5365,22 @@
     </row>
     <row r="63" ht="13.55" customHeight="1">
       <c r="A63" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B63" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C63" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D63" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E63" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F63" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G63" t="s" s="7">
         <v>142</v>
@@ -5410,7 +5414,7 @@
         <v>75</v>
       </c>
       <c r="R63" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S63" t="s" s="10">
         <v>38</v>
@@ -5419,22 +5423,22 @@
     </row>
     <row r="64" ht="13.55" customHeight="1">
       <c r="A64" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B64" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C64" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D64" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E64" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F64" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G64" t="s" s="7">
         <v>142</v>
@@ -5468,7 +5472,7 @@
         <v>75</v>
       </c>
       <c r="R64" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S64" t="s" s="10">
         <v>38</v>
@@ -5477,22 +5481,22 @@
     </row>
     <row r="65" ht="13.55" customHeight="1">
       <c r="A65" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B65" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C65" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D65" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E65" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F65" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G65" t="s" s="7">
         <v>142</v>
@@ -5526,7 +5530,7 @@
         <v>75</v>
       </c>
       <c r="R65" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S65" t="s" s="10">
         <v>38</v>
@@ -5535,22 +5539,22 @@
     </row>
     <row r="66" ht="13.55" customHeight="1">
       <c r="A66" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B66" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C66" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D66" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E66" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F66" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G66" t="s" s="7">
         <v>142</v>
@@ -5584,7 +5588,7 @@
         <v>75</v>
       </c>
       <c r="R66" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S66" t="s" s="10">
         <v>38</v>
@@ -5593,22 +5597,22 @@
     </row>
     <row r="67" ht="13.55" customHeight="1">
       <c r="A67" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B67" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C67" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D67" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E67" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F67" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G67" t="s" s="7">
         <v>142</v>
@@ -5642,7 +5646,7 @@
         <v>75</v>
       </c>
       <c r="R67" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S67" t="s" s="10">
         <v>38</v>
@@ -5651,22 +5655,22 @@
     </row>
     <row r="68" ht="13.55" customHeight="1">
       <c r="A68" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B68" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C68" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D68" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E68" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F68" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G68" t="s" s="7">
         <v>142</v>
@@ -5698,7 +5702,7 @@
       <c r="P68" s="8"/>
       <c r="Q68" s="8"/>
       <c r="R68" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S68" t="s" s="10">
         <v>38</v>
@@ -5707,22 +5711,22 @@
     </row>
     <row r="69" ht="13.55" customHeight="1">
       <c r="A69" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B69" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C69" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D69" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E69" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F69" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G69" t="s" s="7">
         <v>142</v>
@@ -5754,7 +5758,7 @@
       <c r="P69" s="8"/>
       <c r="Q69" s="8"/>
       <c r="R69" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S69" t="s" s="10">
         <v>38</v>
@@ -5763,22 +5767,22 @@
     </row>
     <row r="70" ht="13.55" customHeight="1">
       <c r="A70" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B70" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C70" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D70" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E70" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F70" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G70" t="s" s="7">
         <v>142</v>
@@ -5810,7 +5814,7 @@
       <c r="P70" s="8"/>
       <c r="Q70" s="8"/>
       <c r="R70" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S70" t="s" s="10">
         <v>38</v>
@@ -5819,22 +5823,22 @@
     </row>
     <row r="71" ht="13.55" customHeight="1">
       <c r="A71" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B71" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C71" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D71" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E71" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F71" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G71" t="s" s="7">
         <v>142</v>
@@ -5866,7 +5870,7 @@
       <c r="P71" s="8"/>
       <c r="Q71" s="8"/>
       <c r="R71" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S71" t="s" s="10">
         <v>38</v>
@@ -5875,22 +5879,22 @@
     </row>
     <row r="72" ht="13.55" customHeight="1">
       <c r="A72" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B72" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C72" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D72" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E72" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F72" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G72" t="s" s="7">
         <v>142</v>
@@ -5922,7 +5926,7 @@
       <c r="P72" s="8"/>
       <c r="Q72" s="8"/>
       <c r="R72" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S72" t="s" s="10">
         <v>38</v>
@@ -5931,22 +5935,22 @@
     </row>
     <row r="73" ht="13.55" customHeight="1">
       <c r="A73" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B73" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C73" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D73" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E73" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F73" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G73" t="s" s="7">
         <v>142</v>
@@ -5978,7 +5982,7 @@
       <c r="P73" s="8"/>
       <c r="Q73" s="8"/>
       <c r="R73" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S73" t="s" s="10">
         <v>38</v>
@@ -5987,22 +5991,22 @@
     </row>
     <row r="74" ht="13.55" customHeight="1">
       <c r="A74" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B74" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C74" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D74" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E74" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F74" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G74" t="s" s="7">
         <v>142</v>
@@ -6036,7 +6040,7 @@
         <v>75</v>
       </c>
       <c r="R74" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S74" t="s" s="10">
         <v>38</v>
@@ -6045,22 +6049,22 @@
     </row>
     <row r="75" ht="13.55" customHeight="1">
       <c r="A75" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B75" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C75" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D75" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E75" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F75" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G75" t="s" s="7">
         <v>142</v>
@@ -6092,7 +6096,7 @@
       <c r="P75" s="8"/>
       <c r="Q75" s="8"/>
       <c r="R75" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S75" t="s" s="10">
         <v>38</v>
@@ -6101,22 +6105,22 @@
     </row>
     <row r="76" ht="13.55" customHeight="1">
       <c r="A76" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B76" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C76" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D76" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E76" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F76" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G76" t="s" s="7">
         <v>142</v>
@@ -6148,7 +6152,7 @@
       <c r="P76" s="8"/>
       <c r="Q76" s="8"/>
       <c r="R76" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S76" t="s" s="10">
         <v>38</v>
@@ -6157,22 +6161,22 @@
     </row>
     <row r="77" ht="13.55" customHeight="1">
       <c r="A77" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C77" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D77" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E77" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F77" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G77" t="s" s="7">
         <v>142</v>
@@ -6204,7 +6208,7 @@
       <c r="P77" s="8"/>
       <c r="Q77" s="8"/>
       <c r="R77" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S77" t="s" s="10">
         <v>38</v>
@@ -6213,22 +6217,22 @@
     </row>
     <row r="78" ht="13.55" customHeight="1">
       <c r="A78" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B78" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C78" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D78" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E78" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F78" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G78" t="s" s="7">
         <v>142</v>
@@ -6260,7 +6264,7 @@
       <c r="P78" s="8"/>
       <c r="Q78" s="8"/>
       <c r="R78" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S78" t="s" s="10">
         <v>38</v>
@@ -6269,22 +6273,22 @@
     </row>
     <row r="79" ht="13.55" customHeight="1">
       <c r="A79" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B79" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C79" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D79" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E79" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F79" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G79" t="s" s="7">
         <v>142</v>
@@ -6316,7 +6320,7 @@
       <c r="P79" s="8"/>
       <c r="Q79" s="8"/>
       <c r="R79" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S79" t="s" s="10">
         <v>38</v>
@@ -6325,22 +6329,22 @@
     </row>
     <row r="80" ht="13.55" customHeight="1">
       <c r="A80" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B80" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C80" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D80" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E80" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F80" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G80" t="s" s="7">
         <v>142</v>
@@ -6372,7 +6376,7 @@
       <c r="P80" s="8"/>
       <c r="Q80" s="8"/>
       <c r="R80" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S80" t="s" s="10">
         <v>38</v>
@@ -6381,22 +6385,22 @@
     </row>
     <row r="81" ht="13.55" customHeight="1">
       <c r="A81" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B81" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C81" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D81" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E81" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F81" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G81" t="s" s="7">
         <v>142</v>
@@ -6428,7 +6432,7 @@
       <c r="P81" s="8"/>
       <c r="Q81" s="8"/>
       <c r="R81" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S81" t="s" s="10">
         <v>38</v>
@@ -6437,22 +6441,22 @@
     </row>
     <row r="82" ht="13.55" customHeight="1">
       <c r="A82" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B82" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C82" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D82" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E82" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F82" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G82" t="s" s="7">
         <v>142</v>
@@ -6484,7 +6488,7 @@
       <c r="P82" s="8"/>
       <c r="Q82" s="8"/>
       <c r="R82" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S82" t="s" s="10">
         <v>38</v>
@@ -6493,22 +6497,22 @@
     </row>
     <row r="83" ht="13.55" customHeight="1">
       <c r="A83" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B83" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C83" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D83" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E83" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F83" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G83" t="s" s="7">
         <v>142</v>
@@ -6540,7 +6544,7 @@
       <c r="P83" s="8"/>
       <c r="Q83" s="8"/>
       <c r="R83" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S83" t="s" s="10">
         <v>38</v>
@@ -6549,22 +6553,22 @@
     </row>
     <row r="84" ht="13.55" customHeight="1">
       <c r="A84" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B84" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C84" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D84" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E84" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F84" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G84" t="s" s="7">
         <v>142</v>
@@ -6596,7 +6600,7 @@
       <c r="P84" s="8"/>
       <c r="Q84" s="8"/>
       <c r="R84" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S84" t="s" s="10">
         <v>38</v>
@@ -6605,22 +6609,22 @@
     </row>
     <row r="85" ht="13.55" customHeight="1">
       <c r="A85" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B85" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C85" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D85" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E85" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F85" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G85" t="s" s="7">
         <v>142</v>
@@ -6652,7 +6656,7 @@
       <c r="P85" s="8"/>
       <c r="Q85" s="8"/>
       <c r="R85" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S85" t="s" s="10">
         <v>38</v>
@@ -6661,22 +6665,22 @@
     </row>
     <row r="86" ht="13.55" customHeight="1">
       <c r="A86" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B86" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C86" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D86" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E86" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F86" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G86" t="s" s="7">
         <v>172</v>
@@ -6708,7 +6712,7 @@
       <c r="P86" s="8"/>
       <c r="Q86" s="8"/>
       <c r="R86" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S86" t="s" s="10">
         <v>38</v>
@@ -6717,22 +6721,22 @@
     </row>
     <row r="87" ht="13.55" customHeight="1">
       <c r="A87" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B87" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C87" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D87" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E87" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F87" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G87" t="s" s="7">
         <v>172</v>
@@ -6766,7 +6770,7 @@
         <v>75</v>
       </c>
       <c r="R87" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S87" t="s" s="10">
         <v>38</v>
@@ -6775,22 +6779,22 @@
     </row>
     <row r="88" ht="13.55" customHeight="1">
       <c r="A88" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B88" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C88" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D88" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E88" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F88" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G88" t="s" s="7">
         <v>172</v>
@@ -6826,7 +6830,7 @@
         <v>75</v>
       </c>
       <c r="R88" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S88" t="s" s="10">
         <v>38</v>
@@ -6835,22 +6839,22 @@
     </row>
     <row r="89" ht="13.55" customHeight="1">
       <c r="A89" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B89" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C89" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D89" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E89" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F89" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G89" t="s" s="7">
         <v>172</v>
@@ -6886,7 +6890,7 @@
         <v>75</v>
       </c>
       <c r="R89" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S89" t="s" s="10">
         <v>38</v>
@@ -6895,22 +6899,22 @@
     </row>
     <row r="90" ht="13.55" customHeight="1">
       <c r="A90" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B90" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C90" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D90" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E90" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F90" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G90" t="s" s="7">
         <v>172</v>
@@ -6944,7 +6948,7 @@
         <v>75</v>
       </c>
       <c r="R90" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S90" t="s" s="10">
         <v>38</v>
@@ -6953,22 +6957,22 @@
     </row>
     <row r="91" ht="13.55" customHeight="1">
       <c r="A91" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B91" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C91" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D91" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E91" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F91" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G91" t="s" s="7">
         <v>172</v>
@@ -7000,7 +7004,7 @@
       <c r="P91" s="8"/>
       <c r="Q91" s="8"/>
       <c r="R91" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S91" t="s" s="10">
         <v>38</v>
@@ -7009,22 +7013,22 @@
     </row>
     <row r="92" ht="13.55" customHeight="1">
       <c r="A92" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B92" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C92" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D92" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E92" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F92" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G92" t="s" s="7">
         <v>172</v>
@@ -7056,7 +7060,7 @@
       <c r="P92" s="8"/>
       <c r="Q92" s="8"/>
       <c r="R92" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S92" t="s" s="10">
         <v>38</v>
@@ -7065,22 +7069,22 @@
     </row>
     <row r="93" ht="13.55" customHeight="1">
       <c r="A93" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B93" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C93" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D93" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E93" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F93" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G93" t="s" s="7">
         <v>172</v>
@@ -7112,7 +7116,7 @@
       <c r="P93" s="8"/>
       <c r="Q93" s="8"/>
       <c r="R93" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S93" t="s" s="10">
         <v>38</v>
@@ -7121,22 +7125,22 @@
     </row>
     <row r="94" ht="13.55" customHeight="1">
       <c r="A94" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B94" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C94" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D94" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E94" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F94" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G94" t="s" s="7">
         <v>172</v>
@@ -7168,7 +7172,7 @@
       <c r="P94" s="8"/>
       <c r="Q94" s="8"/>
       <c r="R94" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S94" t="s" s="10">
         <v>38</v>
@@ -7177,22 +7181,22 @@
     </row>
     <row r="95" ht="13.55" customHeight="1">
       <c r="A95" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B95" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C95" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D95" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E95" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F95" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G95" t="s" s="7">
         <v>177</v>
@@ -7224,7 +7228,7 @@
       <c r="P95" s="8"/>
       <c r="Q95" s="8"/>
       <c r="R95" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S95" t="s" s="10">
         <v>38</v>
@@ -7233,22 +7237,22 @@
     </row>
     <row r="96" ht="13.55" customHeight="1">
       <c r="A96" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B96" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C96" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D96" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E96" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F96" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G96" t="s" s="7">
         <v>177</v>
@@ -7282,7 +7286,7 @@
         <v>75</v>
       </c>
       <c r="R96" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S96" t="s" s="10">
         <v>38</v>
@@ -7291,22 +7295,22 @@
     </row>
     <row r="97" ht="13.55" customHeight="1">
       <c r="A97" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B97" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C97" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D97" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E97" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F97" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G97" t="s" s="7">
         <v>177</v>
@@ -7342,7 +7346,7 @@
         <v>75</v>
       </c>
       <c r="R97" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S97" t="s" s="10">
         <v>38</v>
@@ -7351,22 +7355,22 @@
     </row>
     <row r="98" ht="13.55" customHeight="1">
       <c r="A98" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B98" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C98" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D98" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E98" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F98" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G98" t="s" s="7">
         <v>177</v>
@@ -7402,7 +7406,7 @@
         <v>75</v>
       </c>
       <c r="R98" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S98" t="s" s="10">
         <v>38</v>
@@ -7411,22 +7415,22 @@
     </row>
     <row r="99" ht="13.55" customHeight="1">
       <c r="A99" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B99" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C99" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D99" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E99" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F99" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G99" t="s" s="7">
         <v>177</v>
@@ -7460,7 +7464,7 @@
         <v>75</v>
       </c>
       <c r="R99" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S99" t="s" s="10">
         <v>38</v>
@@ -7469,22 +7473,22 @@
     </row>
     <row r="100" ht="13.55" customHeight="1">
       <c r="A100" t="s" s="6">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B100" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C100" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D100" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E100" t="s" s="7">
         <v>23</v>
       </c>
       <c r="F100" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G100" t="s" s="7">
         <v>177</v>
@@ -7516,7 +7520,7 @@
       <c r="P100" s="8"/>
       <c r="Q100" s="8"/>
       <c r="R100" t="s" s="7">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="S100" t="s" s="10">
         <v>38</v>

</xml_diff>